<commit_message>
adding topics to learn into excel
</commit_message>
<xml_diff>
--- a/Git Commands.xlsx
+++ b/Git Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ganeshsha\Desktop\PPP\Github-LearningRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6F7C9A-64CA-4694-85D0-15451D91121B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45C5C46-D65B-4017-91E2-C7DE693AA0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="255" yWindow="135" windowWidth="20235" windowHeight="10785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Scenario</t>
   </si>
@@ -54,29 +54,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Clone:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Copy repository from central/remote/origin to your system</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Pull:</t>
     </r>
     <r>
@@ -102,9 +79,6 @@
 </t>
   </si>
   <si>
-    <t>git init</t>
-  </si>
-  <si>
     <t>1) To initialize existing folder</t>
   </si>
   <si>
@@ -128,29 +102,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Initialising: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>New local repository</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Staging status</t>
     </r>
     <r>
@@ -247,14 +198,57 @@
     <t>1) After executing 2 commands you can see the changes commited to github repository</t>
   </si>
   <si>
-    <t>First create a respository in Github account. Then use below command
-git remote add origin https://github.com/drsladit/MySQL-and-Mongodb-Learning.git
-git push origin master
-and we can use below command to link local master branch to origin master branch
-git push --set-upstream origin master
-to check make changes to file. add, commit and push
-git push
-refresh the page in central repository</t>
+    <t>Case 1: Clone complete github repository to your system</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Case 2: Create new local repository and push changes to github repository
+Initialising: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>New local repository</t>
+    </r>
+  </si>
+  <si>
+    <t>First create a respository in Github account. Then clone the repository from github to your local system.
+git init - if you do not have .git folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git push - will be sufficient.
+</t>
+  </si>
+  <si>
+    <t>Stash</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>commit - soft and hard reset</t>
+  </si>
+  <si>
+    <t>checkout</t>
+  </si>
+  <si>
+    <t>creating new branch</t>
+  </si>
+  <si>
+    <t>How to navigate to existing branch</t>
   </si>
 </sst>
 </file>
@@ -330,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -350,6 +344,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,8 +652,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
+      <c r="A2" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
@@ -665,75 +662,105 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>